<commit_message>
Atualização com conteúdo de post automatizado
</commit_message>
<xml_diff>
--- a/auxiliares/Tabela_produtos.xlsx
+++ b/auxiliares/Tabela_produtos.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanu\Documents\Projeto Afiliados\Lovable_github_CLONE\brincar-com-prop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emanu\Documents\Projeto Afiliados\Lovable_github_CLONE\brincar-com-prop\auxiliares\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0483BA10-A4AD-4CF7-8AEA-300629E54A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDE84BC-DB85-470E-8C65-D6F9E9AE0FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="158">
   <si>
     <t>id</t>
   </si>
@@ -504,6 +505,134 @@
   </si>
   <si>
     <t>A14G98-P634</t>
+  </si>
+  <si>
+    <t>mobile-centopeia</t>
+  </si>
+  <si>
+    <t>Móbile Centopeia Espiral Bebe</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>Mobile Centopeia Espiral Ideal para Carrinho Bebê Conforto Berço, com sons e chocalho.
+Toque macio e confortável, sem riscos para o bebê. Personagens pendurados estimulam o bebê a alcançar, puxar e apertar, contribuindo para o desenvolvimento dos sentidos táteis e coordenação mão-olho.
+Som: Brinquedo com som ao ser apertado, proporcionando ao bebê a descoberta de diferentes sons.</t>
+  </si>
+  <si>
+    <t>https://mercadolivre.com/sec/1XTyNJ7</t>
+  </si>
+  <si>
+    <t>A14G98-JGF5</t>
+  </si>
+  <si>
+    <t>livro-selva</t>
+  </si>
+  <si>
+    <t>Livrinho Jungle</t>
+  </si>
+  <si>
+    <t>O Livrinho de Atividades Jungle Amigos da Selva 15343 da Buba é perfeito para estimular o desenvolvimento dos pequenos desde os 3 meses. Com uma divertida temática de selva, o livrinho oferece uma experiência interativa e educativa para os bebês. Seu design inclui uma base removível e um móbile removível, proporcionando versatilidade e facilidade de uso.
+As atividades presentes no livrinho ajudam a desenvolver habilidades motoras, sensoriais e cognitivas dos bebês, além de estimular a curiosidade e a criatividade. Com ele os bebês poderão explorar diferentes texturas, cores e sons, enquanto se divertem e aprendem.</t>
+  </si>
+  <si>
+    <t>https://mercadolivre.com/sec/21STk9Q</t>
+  </si>
+  <si>
+    <t>A14G98-AGX4</t>
+  </si>
+  <si>
+    <t>coruja-musical</t>
+  </si>
+  <si>
+    <t>Pelúcia Musical Coruja Divertida</t>
+  </si>
+  <si>
+    <t>Não há limites para se divertir com este brinquedo de pelúcia, que será fonte de tranquilidade para as crianças, ajudando-as a desenvolver habilidades sociais, promovendo sua imaginação e criatividade.
+Diversão sem alergias
+A função hipoalergênica permite que as crianças brinquem por horas com o bicho de pelúcia, com a tranquilidade de que os materiais do brinquedo não causarão nenhuma reação alérgica.
+Ilumine suas aventuras
+As luzes do brinquedo de pelúcia lhe acompanharão tanto nas horas de brincadeira como nos momentos de descanso, provocando sonhos fantásticos.
+Potencialize seus sentidos
+Os sons farão com que seu bicho de pelúcia ganhe vida, animando cada momento compartilhado. Escute, ria e dance com o seu novo companheiro de aventuras.</t>
+  </si>
+  <si>
+    <t>https://mercadolivre.com/sec/2h1Bb94</t>
+  </si>
+  <si>
+    <t>A14G98-X4MU</t>
+  </si>
+  <si>
+    <t>tapete-grande-abc</t>
+  </si>
+  <si>
+    <t>https://mercadolivre.com/sec/2MbTkxj</t>
+  </si>
+  <si>
+    <t>A14G98-8W6H</t>
+  </si>
+  <si>
+    <t>Tapete Térmico Estampas Diversas</t>
+  </si>
+  <si>
+    <t>O Tapete Atividades Infantil Bebê Proteção Térmica 1,80X1,20 é perfeito para proporcionar diversão e conforto para o seu bebê. Com estampas variadas e coloridas, esse tapete é muito atrativo para crianças e bebês, estimulando visualmente o seu pequeno e garantindo horas de entretenimento.
+O Tapete Atividades Infantil Bebê Proteção Térmica 1,80X1,20 é durável, educativo e fácil de limpar. Possui forro macio, que proporciona conforto para o bebê durante as atividades. Ele é antialérgico e atóxico, garantindo a segurança do seu filho.
+Com tamanho de 1,80 metros de comprimento por 1,20 metros de largura e espessura de 2,5 mm, esse tapete oferece espaço suficiente para o bebê brincar e se movimentar livremente. Além disso, ele é fácil de transportar, podendo ser levado para qualquer lugar que você precisar.
+Atenção: não é possível escolher a estampa</t>
+  </si>
+  <si>
+    <t>andador-cachorrinho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andador Cachorrinho Fisher-price </t>
+  </si>
+  <si>
+    <t>A diversão dos brinquedos Fisher-Price acompanha o crescimento do seu pequeno e torna cada momento mais leve e repleto de aprendizado!
+ANDADOR CACHORRINHO QUE ANDA.
+Existem 2 maneiras de brincar com o andador conforme o bebê vai crescendo: sentado ou caminhando!
+DIVERSÃO QUE ACOMPANHA SEU BEBÊ.
+Empurrar o Cachorrinho leva o seu bebê a se divertir com as músicas e frases de incentivo. O conteúdo do andador muda conforme a idade e fase do bebê, com a tecnologia Smart Stages!
+ATIVIDADES DE MONTÃO.
+O andador conta com 7 atividades práticas! Teclas de piano, chaves e nariz iluminados, rodas, disco giratório, páginas para virar e muito mais!
+DIVERSIDADE DE SONS.
+Mais de 75 músicas, sons e frases ensinam o alfabeto, formas, cores, números e muito mais neste andador.</t>
+  </si>
+  <si>
+    <t>https://mercadolivre.com/sec/1nsdo37</t>
+  </si>
+  <si>
+    <t>A14G98-T8KK</t>
+  </si>
+  <si>
+    <t>brinquedo-espiral</t>
+  </si>
+  <si>
+    <t>Brinquedo Educativo Paki Rampa</t>
+  </si>
+  <si>
+    <t>Com o Paki Rampa da Paki Toys, vai divertir e entreter a criança enquanto ela aprende e desenvolve seus sentidos. O objetivo é alinhar diversão e aprendizado com segurança. O brinquedo estimula os sentidos tátil e visual e ainda no desenvolvimento da coordenação motora e habilidade manual.</t>
+  </si>
+  <si>
+    <t>https://mercadolivre.com/sec/2W5uGm1</t>
+  </si>
+  <si>
+    <t>A14G98-L62H</t>
+  </si>
+  <si>
+    <t>bate-pino</t>
+  </si>
+  <si>
+    <t>Bate Pino Madeira Infantil Brinquedo Educativo</t>
+  </si>
+  <si>
+    <t>Brinquedo educativo e interativo que estimula a coordenação motora e a percepção visual das crianças. Feito em madeira resistente, possui pinos coloridos para bater e encaixar, proporcionando diversão e aprendizado seguro. Ideal para crianças a partir de 1 ano.</t>
+  </si>
+  <si>
+    <t>https://mercadolivre.com/sec/1TX2ycC</t>
+  </si>
+  <si>
+    <t>A14G98-5JE3</t>
   </si>
 </sst>
 </file>
@@ -565,15 +694,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -878,631 +1008,954 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I18"/>
+      <selection activeCell="A18" sqref="A18:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" t="str">
+      <c r="H2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="1" t="str">
         <f>"./images/"&amp;K2&amp;".png"</f>
         <v>./images/A14G98-YYYK.png</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I18" si="0">"./images/"&amp;K3&amp;".png"</f>
+      <c r="H3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I34" si="0">"./images/"&amp;K3&amp;".png"</f>
         <v>./images/A14G98-LES9.png</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" t="str">
+      <c r="H4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-5SDW.png</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" t="str">
+      <c r="H5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-AV2X.png</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" t="str">
+      <c r="H6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-H4C4.png</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I7" t="str">
+      <c r="I7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-6A46.png</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I8" t="str">
+      <c r="I8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-NTWS.png</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H9" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" t="str">
+      <c r="H9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-5WAB.png</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" t="str">
+      <c r="H10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-6B7C.png</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="H11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" t="str">
+      <c r="H11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-9TSN.png</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" t="str">
+      <c r="H12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-0Q7X.png</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H13" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" t="str">
+      <c r="H13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-GBM3.png</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H14" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" t="str">
+      <c r="H14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-HV5X.png</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H15" t="s">
-        <v>76</v>
-      </c>
-      <c r="I15" t="str">
+      <c r="H15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-4GX5.png</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H16" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" t="str">
+      <c r="H16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-3VT8.png</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" t="str">
+      <c r="H17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-97YL.png</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K17" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H18" t="s">
-        <v>76</v>
-      </c>
-      <c r="I18" t="str">
+      <c r="H18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>./images/A14G98-P634.png</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/A14G98-JGF5.png</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="1" t="str">
+        <f>A20</f>
+        <v>livro-selva</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/A14G98-AGX4.png</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="1" t="str">
+        <f t="shared" ref="C21:C34" si="1">A21</f>
+        <v>coruja-musical</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/A14G98-X4MU.png</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>tapete-grande-abc</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/A14G98-8W6H.png</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>andador-cachorrinho</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/A14G98-T8KK.png</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>brinquedo-espiral</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/A14G98-L62H.png</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>bate-pino</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/A14G98-5JE3.png</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/.png</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/.png</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/.png</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/.png</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/.png</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/.png</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/.png</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/.png</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>./images/.png</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1085BD-49C1-486F-A74B-16FC4D6615E0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>